<commit_message>
Dialog from Excel file
</commit_message>
<xml_diff>
--- a/ss/MateRun3_2/MAZE RUN 3/Assets/Scripts/Excel-Daten-MR.xlsx
+++ b/ss/MateRun3_2/MAZE RUN 3/Assets/Scripts/Excel-Daten-MR.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://htlr-my.sharepoint.com/personal/semih_soenmez_student_htl-rankweil_at/Documents/Dokumente/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HTL_2021-22\Diplomarbeit\DA--MazeRun2\ss\MateRun3_2\MAZE RUN 3\Assets\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB4C369D-3B4F-4EBE-B618-5FFD80E45637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90E7578-3101-4206-A2B5-DB4B11117094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7F51EEE9-8E90-4834-9E91-E5A130D44FD7}"/>
   </bookViews>
@@ -34,12 +34,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>sentences</t>
   </si>
   <si>
     <t>charakter</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>c3</t>
+  </si>
+  <si>
+    <t>s1</t>
+  </si>
+  <si>
+    <t>s2</t>
+  </si>
+  <si>
+    <t>s3</t>
   </si>
 </sst>
 </file>
@@ -391,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0E45AD-8329-49B9-835D-D752FF816204}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,6 +425,30 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>